<commit_message>
Update figure 1 and results
</commit_message>
<xml_diff>
--- a/Table_S1.xlsx
+++ b/Table_S1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Small_plasmid_Nanopore/GitHub_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78B82D-785D-5542-B4F7-CE4EEB811B89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DAA6E0-CE7B-F743-924B-4A205B296504}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6600" yWindow="-25260" windowWidth="31300" windowHeight="19020" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
+    <workbookView xWindow="2760" yWindow="-25280" windowWidth="31300" windowHeight="19020" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet descriptions" sheetId="5" r:id="rId1"/>
@@ -2737,7 +2737,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add some explanatory comments
</commit_message>
<xml_diff>
--- a/Table_S1.xlsx
+++ b/Table_S1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Small_plasmid_Nanopore/GitHub_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262F6949-DBDC-8D47-8B92-838C3CA7BFB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC09EF64-EC64-4B40-A49E-E4BE99519CE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="-27080" windowWidth="35520" windowHeight="25160" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
+    <workbookView xWindow="1440" yWindow="-27560" windowWidth="35520" windowHeight="25160" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet descriptions" sheetId="5" r:id="rId1"/>
@@ -62,7 +62,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Since not all runs lasted the same time and some involved refueling, this column shows the yield of only the first 12 hours of sequencing.</t>
+    Since not all runs lasted the same time and some involved refuelling, this column shows the yield of only the first 12 hours of sequencing. This allows for easier comparison of run yields.</t>
       </text>
     </comment>
     <comment ref="H1" authorId="2" shapeId="0" xr:uid="{1BCA6B03-9B93-2745-B715-C3D66DE583A1}">
@@ -120,7 +120,35 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={0A0896FA-E917-9B46-A4F1-1EC9E3225999}</author>
+    <author>tc={9CBC07C7-BCD3-4A4E-930D-917AEB118324}</author>
+  </authors>
+  <commentList>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{0A0896FA-E917-9B46-A4F1-1EC9E3225999}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Determined computationally by aligning the reads to the assembly and taking the insert sizes from the resulting BAM file.</t>
+      </text>
+    </comment>
+    <comment ref="AC1" authorId="1" shapeId="0" xr:uid="{9CBC07C7-BCD3-4A4E-930D-917AEB118324}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Determined computationally by aligning the reads to the assembly and taking the insert sizes from the resulting BAM file.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={A4FEB2D8-86B2-C243-B0A2-060A3B2D97BF}</author>
+    <author>tc={0672B199-9508-F641-9015-B2DD53AAB038}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A4FEB2D8-86B2-C243-B0A2-060A3B2D97BF}">
@@ -128,8 +156,17 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Since the two technical replicates used separate cultures and DNA extractions, per-replicon read depth values are specific to the technical replicate.
+    Technical replicate 1 includes ligation run 1 and rapid run 1. Technical replicate 2 includes ligation run 2 and rapid run 2.
+Since the two technical replicates used separate cultures and DNA extractions, per-replicon read depth values are specific to the technical replicate.
 For example, the depth of A. baumannii J9 plasmid_1 could be different in the two replicates and therefore needs two separate lines in this table.</t>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="1" shapeId="0" xr:uid="{0672B199-9508-F641-9015-B2DD53AAB038}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    See the ‘Notes’ worksheet for detailed explanations.</t>
       </text>
     </comment>
   </commentList>
@@ -778,7 +815,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -828,6 +865,12 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1750,7 +1793,7 @@
     <text>This is the total yield of the run, including reads from all barcodes (even unused ones) and unclassified reads.</text>
   </threadedComment>
   <threadedComment ref="C1" dT="2020-10-08T23:17:29.04" personId="{ECA94A02-CA93-664F-B733-A1DC520C84D0}" id="{0F82EF9B-2018-3449-9FDD-397D5647740F}">
-    <text>Since not all runs lasted the same time and some involved refueling, this column shows the yield of only the first 12 hours of sequencing.</text>
+    <text>Since not all runs lasted the same time and some involved refuelling, this column shows the yield of only the first 12 hours of sequencing. This allows for easier comparison of run yields.</text>
   </threadedComment>
   <threadedComment ref="H1" dT="2020-10-02T00:41:34.42" personId="{ECA94A02-CA93-664F-B733-A1DC520C84D0}" id="{1BCA6B03-9B93-2745-B715-C3D66DE583A1}">
     <text>This is the fraction of reads that are chimeras within a single barcode bin. For example, a read which is half from a chromosome and half from a plasmid of the same genome.</text>
@@ -1775,9 +1818,24 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="P1" dT="2021-02-01T00:52:24.46" personId="{ECA94A02-CA93-664F-B733-A1DC520C84D0}" id="{0A0896FA-E917-9B46-A4F1-1EC9E3225999}">
+    <text>Determined computationally by aligning the reads to the assembly and taking the insert sizes from the resulting BAM file.</text>
+  </threadedComment>
+  <threadedComment ref="AC1" dT="2021-02-01T00:52:29.17" personId="{ECA94A02-CA93-664F-B733-A1DC520C84D0}" id="{9CBC07C7-BCD3-4A4E-930D-917AEB118324}">
+    <text>Determined computationally by aligning the reads to the assembly and taking the insert sizes from the resulting BAM file.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2020-10-02T00:49:59.97" personId="{ECA94A02-CA93-664F-B733-A1DC520C84D0}" id="{A4FEB2D8-86B2-C243-B0A2-060A3B2D97BF}">
-    <text>Since the two technical replicates used separate cultures and DNA extractions, per-replicon read depth values are specific to the technical replicate.
+    <text>Technical replicate 1 includes ligation run 1 and rapid run 1. Technical replicate 2 includes ligation run 2 and rapid run 2.
+Since the two technical replicates used separate cultures and DNA extractions, per-replicon read depth values are specific to the technical replicate.
 For example, the depth of A. baumannii J9 plasmid_1 could be different in the two replicates and therefore needs two separate lines in this table.</text>
+  </threadedComment>
+  <threadedComment ref="Q1" dT="2021-02-01T00:54:15.32" personId="{ECA94A02-CA93-664F-B733-A1DC520C84D0}" id="{0672B199-9508-F641-9015-B2DD53AAB038}">
+    <text>See the ‘Notes’ worksheet for detailed explanations.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2038,7 +2096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45BD62-7DEE-0740-97DB-27A0DE7F03FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D45BD62-7DEE-0740-97DB-27A0DE7F03FC}">
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -3031,6 +3089,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Kleborate results to Table S1
</commit_message>
<xml_diff>
--- a/Table_S1.xlsx
+++ b/Table_S1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Small_plasmid_Nanopore/GitHub_repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Small_plasmid_Nanopore/Paper_GitHub_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC09EF64-EC64-4B40-A49E-E4BE99519CE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C36DDB-5118-E444-B125-697ADDA2600E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="-27560" windowWidth="35520" windowHeight="25160" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
   </bookViews>
@@ -18,8 +18,9 @@
     <sheet name="Per-barcode" sheetId="1" r:id="rId3"/>
     <sheet name="Per-replicon" sheetId="2" r:id="rId4"/>
     <sheet name="Notes" sheetId="4" r:id="rId5"/>
+    <sheet name="Kleborate results" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -174,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="143">
   <si>
     <t>Genome</t>
   </si>
@@ -805,6 +806,221 @@
       <t xml:space="preserve"> worksheet, e.g. a reason for exclusion.</t>
     </r>
   </si>
+  <si>
+    <t>Acinetobacter_baumannii_J9__006078</t>
+  </si>
+  <si>
+    <t>ant(2'')-Ia*</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Acinetobacter_baumannii_J9__145059</t>
+  </si>
+  <si>
+    <t>mphE.v2;msrE</t>
+  </si>
+  <si>
+    <t>floR.v2*</t>
+  </si>
+  <si>
+    <t>sul2^</t>
+  </si>
+  <si>
+    <t>ADC-10*</t>
+  </si>
+  <si>
+    <t>Citrobacter_koseri_MINF_9D__009294</t>
+  </si>
+  <si>
+    <t>Citrobacter_koseri_MINF_9D__064962</t>
+  </si>
+  <si>
+    <t>CTX-M-15</t>
+  </si>
+  <si>
+    <t>TEM-141*?-0%</t>
+  </si>
+  <si>
+    <t>Enterobacter_kobei_MSB1_1B__002369</t>
+  </si>
+  <si>
+    <t>Enterobacter_kobei_MSB1_1B__003715</t>
+  </si>
+  <si>
+    <t>Enterobacter_kobei_MSB1_1B__004665</t>
+  </si>
+  <si>
+    <t>Enterobacter_kobei_MSB1_1B__108411</t>
+  </si>
+  <si>
+    <t>Enterobacter_kobei_MSB1_1B__136482</t>
+  </si>
+  <si>
+    <t>Haemophilus_unknown_M1C132_1__005675</t>
+  </si>
+  <si>
+    <t>Haemophilus_unknown_M1C132_1__007392</t>
+  </si>
+  <si>
+    <t>Haemophilus_unknown_M1C132_1__009975</t>
+  </si>
+  <si>
+    <t>TEM-1D.v1^</t>
+  </si>
+  <si>
+    <t>Haemophilus_unknown_M1C132_1__010719</t>
+  </si>
+  <si>
+    <t>Haemophilus_unknown_M1C132_1__039398</t>
+  </si>
+  <si>
+    <t>Klebsiella_oxytoca_MSB1_2C__004574</t>
+  </si>
+  <si>
+    <t>Klebsiella_oxytoca_MSB1_2C__009975</t>
+  </si>
+  <si>
+    <t>Klebsiella_oxytoca_MSB1_2C__058472</t>
+  </si>
+  <si>
+    <t>Klebsiella_oxytoca_MSB1_2C__118161</t>
+  </si>
+  <si>
+    <t>Klebsiella_variicola_INF345__003514</t>
+  </si>
+  <si>
+    <t>Klebsiella_variicola_INF345__005783</t>
+  </si>
+  <si>
+    <t>Klebsiella_variicola_INF345__031780</t>
+  </si>
+  <si>
+    <t>Klebsiella_variicola_INF345__243620</t>
+  </si>
+  <si>
+    <t>aac(6')-Ib-cr.v2;strA.v1^;strB.v1</t>
+  </si>
+  <si>
+    <t>qnrB1.v2^</t>
+  </si>
+  <si>
+    <t>CatB4.v1</t>
+  </si>
+  <si>
+    <t>sul2</t>
+  </si>
+  <si>
+    <t>tet(A).v1</t>
+  </si>
+  <si>
+    <t>dfrA14.v2*</t>
+  </si>
+  <si>
+    <t>OXA-1;TEM-1D.v1^</t>
+  </si>
+  <si>
+    <t>Klebsiella_variicola_INF345__250980</t>
+  </si>
+  <si>
+    <t>Serratia_marcescens_17-147-1671__001934</t>
+  </si>
+  <si>
+    <t>Serratia_marcescens_17-147-1671__017406</t>
+  </si>
+  <si>
+    <t>Serratia_marcescens_17-147-1671__161385</t>
+  </si>
+  <si>
+    <t>aac(6')-Ib4</t>
+  </si>
+  <si>
+    <t>catB3.v2</t>
+  </si>
+  <si>
+    <t>sul1</t>
+  </si>
+  <si>
+    <t>IMP-4</t>
+  </si>
+  <si>
+    <t>Serratia_marcescens_17-147-1671__184477</t>
+  </si>
+  <si>
+    <t>Plasmid</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kleborate results</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> worksheet contains the Kleborate gene search results for each plasmid, with empty columns removed. Any plasmid which contains at least one resistance gene is highlighted in yellow.</t>
+    </r>
+  </si>
+  <si>
+    <t>resistance score</t>
+  </si>
+  <si>
+    <t>num resistance classes</t>
+  </si>
+  <si>
+    <t>num resistance genes</t>
+  </si>
+  <si>
+    <t>AGly acquired</t>
+  </si>
+  <si>
+    <t>Flq acquired</t>
+  </si>
+  <si>
+    <t>MLS acquired</t>
+  </si>
+  <si>
+    <t>Phe acquired</t>
+  </si>
+  <si>
+    <t>Sul acquired</t>
+  </si>
+  <si>
+    <t>Tet acquired</t>
+  </si>
+  <si>
+    <t>Tmt acquired</t>
+  </si>
+  <si>
+    <t>Bla acquired</t>
+  </si>
+  <si>
+    <t>Bla inhR acquired</t>
+  </si>
+  <si>
+    <t>Bla ESBL acquired</t>
+  </si>
+  <si>
+    <t>Bla Carb acquired</t>
+  </si>
+  <si>
+    <t>truncated resistance hits</t>
+  </si>
 </sst>
 </file>
 
@@ -868,13 +1084,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -899,8 +1116,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1113,11 +1336,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1462,6 +1718,28 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="45"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1842,7 +2120,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0DFF7C-C846-D14B-915D-C0573D580EBA}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1864,6 +2142,11 @@
     <row r="5" spans="1:1" ht="134" x14ac:dyDescent="0.25">
       <c r="A5" s="88" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="66" x14ac:dyDescent="0.25">
+      <c r="A7" s="88" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -6319,4 +6602,1429 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D58F08-71C4-B940-847D-1372352C8926}">
+  <dimension ref="A1:P28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.1640625" style="56" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="56" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.83203125" style="56" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="176" customFormat="1" ht="135" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="175" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="173" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="174">
+        <v>0</v>
+      </c>
+      <c r="C2" s="174">
+        <v>1</v>
+      </c>
+      <c r="D2" s="174">
+        <v>1</v>
+      </c>
+      <c r="E2" s="174" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="M2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="O2" s="174" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" s="174" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="169" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="170">
+        <v>1</v>
+      </c>
+      <c r="C3" s="170">
+        <v>4</v>
+      </c>
+      <c r="D3" s="170">
+        <v>5</v>
+      </c>
+      <c r="E3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="170" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="170" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="170" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="N3" s="170" t="s">
+        <v>86</v>
+      </c>
+      <c r="O3" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="170" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="167" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="168">
+        <v>0</v>
+      </c>
+      <c r="C4" s="168">
+        <v>0</v>
+      </c>
+      <c r="D4" s="168">
+        <v>0</v>
+      </c>
+      <c r="E4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P4" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="169" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="170">
+        <v>1</v>
+      </c>
+      <c r="C5" s="170">
+        <v>1</v>
+      </c>
+      <c r="D5" s="170">
+        <v>1</v>
+      </c>
+      <c r="E5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" s="170" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" s="170" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="167" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="168">
+        <v>0</v>
+      </c>
+      <c r="C6" s="168">
+        <v>0</v>
+      </c>
+      <c r="D6" s="168">
+        <v>0</v>
+      </c>
+      <c r="E6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O6" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P6" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="167" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="168">
+        <v>0</v>
+      </c>
+      <c r="C7" s="168">
+        <v>0</v>
+      </c>
+      <c r="D7" s="168">
+        <v>0</v>
+      </c>
+      <c r="E7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O7" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P7" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="167" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="168">
+        <v>0</v>
+      </c>
+      <c r="C8" s="168">
+        <v>0</v>
+      </c>
+      <c r="D8" s="168">
+        <v>0</v>
+      </c>
+      <c r="E8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P8" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="167" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="168">
+        <v>0</v>
+      </c>
+      <c r="C9" s="168">
+        <v>0</v>
+      </c>
+      <c r="D9" s="168">
+        <v>0</v>
+      </c>
+      <c r="E9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P9" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="167" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="168">
+        <v>0</v>
+      </c>
+      <c r="C10" s="168">
+        <v>0</v>
+      </c>
+      <c r="D10" s="168">
+        <v>0</v>
+      </c>
+      <c r="E10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="167" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="168">
+        <v>0</v>
+      </c>
+      <c r="C11" s="168">
+        <v>0</v>
+      </c>
+      <c r="D11" s="168">
+        <v>0</v>
+      </c>
+      <c r="E11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="167" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="168">
+        <v>0</v>
+      </c>
+      <c r="C12" s="168">
+        <v>0</v>
+      </c>
+      <c r="D12" s="168">
+        <v>0</v>
+      </c>
+      <c r="E12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P12" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="169" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="170">
+        <v>0</v>
+      </c>
+      <c r="C13" s="170">
+        <v>1</v>
+      </c>
+      <c r="D13" s="170">
+        <v>1</v>
+      </c>
+      <c r="E13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="L13" s="170" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="O13" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="P13" s="170" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="167" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="168">
+        <v>0</v>
+      </c>
+      <c r="C14" s="168">
+        <v>0</v>
+      </c>
+      <c r="D14" s="168">
+        <v>0</v>
+      </c>
+      <c r="E14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P14" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="167" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="168">
+        <v>0</v>
+      </c>
+      <c r="C15" s="168">
+        <v>0</v>
+      </c>
+      <c r="D15" s="168">
+        <v>0</v>
+      </c>
+      <c r="E15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P15" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="167" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="168">
+        <v>0</v>
+      </c>
+      <c r="C16" s="168">
+        <v>0</v>
+      </c>
+      <c r="D16" s="168">
+        <v>0</v>
+      </c>
+      <c r="E16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O16" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P16" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="169" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="170">
+        <v>0</v>
+      </c>
+      <c r="C17" s="170">
+        <v>1</v>
+      </c>
+      <c r="D17" s="170">
+        <v>1</v>
+      </c>
+      <c r="E17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="K17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="L17" s="170" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="N17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="O17" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="P17" s="170" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="167" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="168">
+        <v>0</v>
+      </c>
+      <c r="C18" s="168">
+        <v>0</v>
+      </c>
+      <c r="D18" s="168">
+        <v>0</v>
+      </c>
+      <c r="E18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O18" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P18" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="167" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="168">
+        <v>0</v>
+      </c>
+      <c r="C19" s="168">
+        <v>0</v>
+      </c>
+      <c r="D19" s="168">
+        <v>0</v>
+      </c>
+      <c r="E19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P19" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="167" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="168">
+        <v>0</v>
+      </c>
+      <c r="C20" s="168">
+        <v>0</v>
+      </c>
+      <c r="D20" s="168">
+        <v>0</v>
+      </c>
+      <c r="E20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O20" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P20" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="167" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="168">
+        <v>0</v>
+      </c>
+      <c r="C21" s="168">
+        <v>0</v>
+      </c>
+      <c r="D21" s="168">
+        <v>0</v>
+      </c>
+      <c r="E21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O21" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P21" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="167" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" s="168">
+        <v>0</v>
+      </c>
+      <c r="C22" s="168">
+        <v>0</v>
+      </c>
+      <c r="D22" s="168">
+        <v>0</v>
+      </c>
+      <c r="E22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O22" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P22" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="169" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="170">
+        <v>1</v>
+      </c>
+      <c r="C23" s="170">
+        <v>8</v>
+      </c>
+      <c r="D23" s="170">
+        <v>11</v>
+      </c>
+      <c r="E23" s="170" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="170" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="170" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23" s="170" t="s">
+        <v>113</v>
+      </c>
+      <c r="J23" s="170" t="s">
+        <v>114</v>
+      </c>
+      <c r="K23" s="170" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="170" t="s">
+        <v>116</v>
+      </c>
+      <c r="M23" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="N23" s="170" t="s">
+        <v>89</v>
+      </c>
+      <c r="O23" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="P23" s="170" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" s="167" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="168">
+        <v>0</v>
+      </c>
+      <c r="C24" s="168">
+        <v>0</v>
+      </c>
+      <c r="D24" s="168">
+        <v>0</v>
+      </c>
+      <c r="E24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O24" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P24" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" s="167" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="168">
+        <v>0</v>
+      </c>
+      <c r="C25" s="168">
+        <v>0</v>
+      </c>
+      <c r="D25" s="168">
+        <v>0</v>
+      </c>
+      <c r="E25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O25" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P25" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="167" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="168">
+        <v>0</v>
+      </c>
+      <c r="C26" s="168">
+        <v>0</v>
+      </c>
+      <c r="D26" s="168">
+        <v>0</v>
+      </c>
+      <c r="E26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="K26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="L26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="M26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="N26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="O26" s="168" t="s">
+        <v>81</v>
+      </c>
+      <c r="P26" s="168" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="169" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="170">
+        <v>2</v>
+      </c>
+      <c r="C27" s="170">
+        <v>5</v>
+      </c>
+      <c r="D27" s="170">
+        <v>5</v>
+      </c>
+      <c r="E27" s="170" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="H27" s="170" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="170" t="s">
+        <v>123</v>
+      </c>
+      <c r="J27" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="L27" s="170" t="s">
+        <v>99</v>
+      </c>
+      <c r="M27" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="N27" s="170" t="s">
+        <v>81</v>
+      </c>
+      <c r="O27" s="170" t="s">
+        <v>124</v>
+      </c>
+      <c r="P27" s="170" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="171" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="172">
+        <v>0</v>
+      </c>
+      <c r="C28" s="172">
+        <v>1</v>
+      </c>
+      <c r="D28" s="172">
+        <v>1</v>
+      </c>
+      <c r="E28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="H28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="L28" s="172" t="s">
+        <v>99</v>
+      </c>
+      <c r="M28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="N28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="O28" s="172" t="s">
+        <v>81</v>
+      </c>
+      <c r="P28" s="172" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix issue with contaminant plasmid
</commit_message>
<xml_diff>
--- a/Table_S1.xlsx
+++ b/Table_S1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Small_plasmid_Nanopore/Paper_GitHub_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44FBEC0-9B3A-E841-AE48-3138C650F3BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69644BBD-8AC0-3B48-9A2D-1A3462807957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6240" yWindow="-26900" windowWidth="29500" windowHeight="23660" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
+    <workbookView xWindow="4220" yWindow="-21980" windowWidth="36660" windowHeight="20680" xr2:uid="{03D76918-5CA6-BC4B-A785-F8ABEB5E7723}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet descriptions" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Notes" sheetId="4" r:id="rId5"/>
     <sheet name="Kleborate results" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2123,13 +2123,13 @@
       </c>
       <c r="K2" s="89"/>
       <c r="L2" s="89">
-        <v>6.6381580000000004E-6</v>
+        <v>6.6413250000000003E-6</v>
       </c>
       <c r="M2" s="89">
-        <v>2.2154E-2</v>
+        <v>2.2162669570000001E-2</v>
       </c>
       <c r="N2" s="89">
-        <v>2.2160639999999999E-2</v>
+        <v>2.2169310894E-2</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2163,13 +2163,13 @@
       </c>
       <c r="K3" s="97"/>
       <c r="L3" s="97">
-        <v>6.252016E-6</v>
+        <v>6.2536349999999996E-6</v>
       </c>
       <c r="M3" s="97">
-        <v>2.9251929999999999E-2</v>
+        <v>2.9236994002999998E-2</v>
       </c>
       <c r="N3" s="97">
-        <v>2.925819E-2</v>
+        <v>2.9243247638E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2203,13 +2203,13 @@
       </c>
       <c r="K4" s="93"/>
       <c r="L4" s="93">
-        <v>5.6571279999999995E-4</v>
+        <v>5.6321759999999996E-4</v>
       </c>
       <c r="M4" s="93">
-        <v>3.3300320000000001E-3</v>
+        <v>3.336257E-3</v>
       </c>
       <c r="N4" s="93">
-        <v>3.8957449999999999E-3</v>
+        <v>3.8994746000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2243,13 +2243,13 @@
       </c>
       <c r="K5" s="101"/>
       <c r="L5" s="101">
-        <v>5.8573369999999998E-4</v>
+        <v>5.8569959999999995E-4</v>
       </c>
       <c r="M5" s="101">
-        <v>3.8229289999999999E-2</v>
+        <v>3.8117327300000003E-2</v>
       </c>
       <c r="N5" s="101">
-        <v>3.881503E-2</v>
+        <v>3.87030269E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5413,7 +5413,7 @@
         <v>597.79049029999999</v>
       </c>
       <c r="I47" s="65">
-        <f>H47/H$47</f>
+        <f t="shared" ref="I47:I52" si="12">H47/H$47</f>
         <v>1</v>
       </c>
       <c r="J47" s="65"/>
@@ -5421,7 +5421,7 @@
         <v>581.09536179999998</v>
       </c>
       <c r="L47" s="65">
-        <f>K47/K$47</f>
+        <f t="shared" ref="L47:L52" si="13">K47/K$47</f>
         <v>1</v>
       </c>
       <c r="M47" s="65"/>
@@ -5429,7 +5429,7 @@
         <v>155.8212652</v>
       </c>
       <c r="O47" s="65">
-        <f>N47/N$47</f>
+        <f t="shared" ref="O47:O52" si="14">N47/N$47</f>
         <v>1</v>
       </c>
       <c r="P47" s="65"/>
@@ -5459,7 +5459,7 @@
         <v>2643.065486</v>
       </c>
       <c r="I48" s="66">
-        <f>H48/H$47</f>
+        <f t="shared" si="12"/>
         <v>4.4213909871225665</v>
       </c>
       <c r="J48" s="66"/>
@@ -5467,7 +5467,7 @@
         <v>642.99733490000006</v>
       </c>
       <c r="L48" s="66">
-        <f>K48/K$47</f>
+        <f t="shared" si="13"/>
         <v>1.1065263589581109</v>
       </c>
       <c r="M48" s="66"/>
@@ -5475,7 +5475,7 @@
         <v>391.10541139999998</v>
       </c>
       <c r="O48" s="66">
-        <f>N48/N$47</f>
+        <f t="shared" si="14"/>
         <v>2.5099617237609233</v>
       </c>
       <c r="P48" s="66"/>
@@ -5505,7 +5505,7 @@
         <v>14502.741770000001</v>
       </c>
       <c r="I49" s="66">
-        <f>H49/H$47</f>
+        <f t="shared" si="12"/>
         <v>24.260576247577688</v>
       </c>
       <c r="J49" s="66"/>
@@ -5513,7 +5513,7 @@
         <v>1019.1577569999999</v>
       </c>
       <c r="L49" s="66">
-        <f>K49/K$47</f>
+        <f t="shared" si="13"/>
         <v>1.7538562927830961</v>
       </c>
       <c r="M49" s="66"/>
@@ -5521,7 +5521,7 @@
         <v>2372.5406290000001</v>
       </c>
       <c r="O49" s="66">
-        <f>N49/N$47</f>
+        <f t="shared" si="14"/>
         <v>15.226038794864053</v>
       </c>
       <c r="P49" s="66"/>
@@ -5551,7 +5551,7 @@
         <v>20669.93548</v>
       </c>
       <c r="I50" s="66">
-        <f>H50/H$47</f>
+        <f t="shared" si="12"/>
         <v>34.577223651762736</v>
       </c>
       <c r="J50" s="168"/>
@@ -5559,7 +5559,7 @@
         <v>2836.9639590000002</v>
       </c>
       <c r="L50" s="66">
-        <f>K50/K$47</f>
+        <f t="shared" si="13"/>
         <v>4.8820970627131244</v>
       </c>
       <c r="M50" s="168"/>
@@ -5567,7 +5567,7 @@
         <v>3315.9745119999998</v>
       </c>
       <c r="O50" s="66">
-        <f>N50/N$47</f>
+        <f t="shared" si="14"/>
         <v>21.280628852190837</v>
       </c>
       <c r="P50" s="167"/>
@@ -5597,7 +5597,7 @@
         <v>337.79044909999999</v>
       </c>
       <c r="I51" s="66">
-        <f>H51/H$47</f>
+        <f t="shared" si="12"/>
         <v>0.56506494261974716</v>
       </c>
       <c r="J51" s="66"/>
@@ -5605,7 +5605,7 @@
         <v>16.356331170000001</v>
       </c>
       <c r="L51" s="66">
-        <f>K51/K$47</f>
+        <f t="shared" si="13"/>
         <v>2.8147413049959061E-2</v>
       </c>
       <c r="M51" s="66"/>
@@ -5613,7 +5613,7 @@
         <v>43.190205630000001</v>
       </c>
       <c r="O51" s="66">
-        <f>N51/N$47</f>
+        <f t="shared" si="14"/>
         <v>0.27717786513005416</v>
       </c>
       <c r="P51" s="66"/>
@@ -5643,7 +5643,7 @@
         <v>546.37039649999997</v>
       </c>
       <c r="I52" s="67">
-        <f>H52/H$47</f>
+        <f t="shared" si="12"/>
         <v>0.9139830849865227</v>
       </c>
       <c r="J52" s="67"/>
@@ -5651,7 +5651,7 @@
         <v>12.35594714</v>
       </c>
       <c r="L52" s="67">
-        <f>K52/K$47</f>
+        <f t="shared" si="13"/>
         <v>2.1263200418131439E-2</v>
       </c>
       <c r="M52" s="67"/>
@@ -5659,7 +5659,7 @@
         <v>79.194537440000005</v>
       </c>
       <c r="O52" s="67">
-        <f>N52/N$47</f>
+        <f t="shared" si="14"/>
         <v>0.50823959963585252</v>
       </c>
       <c r="P52" s="67"/>
@@ -5873,7 +5873,7 @@
         <v>219.1897644</v>
       </c>
       <c r="I57" s="65">
-        <f t="shared" ref="I57:I62" si="12">H57/H$57</f>
+        <f t="shared" ref="I57:I62" si="15">H57/H$57</f>
         <v>1</v>
       </c>
       <c r="J57" s="65"/>
@@ -5881,7 +5881,7 @@
         <v>296.75099460000001</v>
       </c>
       <c r="L57" s="65">
-        <f t="shared" ref="L57:L62" si="13">K57/K$57</f>
+        <f t="shared" ref="L57:L62" si="16">K57/K$57</f>
         <v>1</v>
       </c>
       <c r="M57" s="65"/>
@@ -5889,7 +5889,7 @@
         <v>80.038454119999997</v>
       </c>
       <c r="O57" s="65">
-        <f t="shared" ref="O57:O62" si="14">N57/N$57</f>
+        <f t="shared" ref="O57:O62" si="17">N57/N$57</f>
         <v>1</v>
       </c>
       <c r="P57" s="65"/>
@@ -5919,7 +5919,7 @@
         <v>136.9907082</v>
       </c>
       <c r="I58" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.62498679431948878</v>
       </c>
       <c r="J58" s="66"/>
@@ -5927,7 +5927,7 @@
         <v>110.6715269</v>
       </c>
       <c r="L58" s="66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.37294408077444741</v>
       </c>
       <c r="M58" s="66"/>
@@ -5935,7 +5935,7 @@
         <v>41.364738750000001</v>
       </c>
       <c r="O58" s="66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.51681081556101405</v>
       </c>
       <c r="P58" s="66"/>
@@ -5965,7 +5965,7 @@
         <v>150.1272567</v>
       </c>
       <c r="I59" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.68491910245422027</v>
       </c>
       <c r="J59" s="66"/>
@@ -5973,7 +5973,7 @@
         <v>160.86113570000001</v>
       </c>
       <c r="L59" s="66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.542074461845797</v>
       </c>
       <c r="M59" s="66"/>
@@ -5981,7 +5981,7 @@
         <v>52.478047310000001</v>
       </c>
       <c r="O59" s="66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.65566043081392789</v>
       </c>
       <c r="P59" s="66"/>
@@ -6011,7 +6011,7 @@
         <v>953.63005029999999</v>
       </c>
       <c r="I60" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>4.3507052115796698</v>
       </c>
       <c r="J60" s="66"/>
@@ -6019,7 +6019,7 @@
         <v>239.71834490000001</v>
       </c>
       <c r="L60" s="66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.8078097437318581</v>
       </c>
       <c r="M60" s="66"/>
@@ -6027,7 +6027,7 @@
         <v>399.10113280000002</v>
       </c>
       <c r="O60" s="66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>4.9863673304039073</v>
       </c>
       <c r="P60" s="66"/>
@@ -6057,7 +6057,7 @@
         <v>2942.0133150000001</v>
       </c>
       <c r="I61" s="66">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>13.42222034433648</v>
       </c>
       <c r="J61" s="66"/>
@@ -6065,7 +6065,7 @@
         <v>312.9991354</v>
       </c>
       <c r="L61" s="66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1.0547534501843923</v>
       </c>
       <c r="M61" s="66"/>
@@ -6073,7 +6073,7 @@
         <v>749.06259729999999</v>
       </c>
       <c r="O61" s="66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9.3587839187516781</v>
       </c>
       <c r="P61" s="66"/>
@@ -6103,7 +6103,7 @@
         <v>1927.2068870000001</v>
       </c>
       <c r="I62" s="67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>8.7924127856765928</v>
       </c>
       <c r="J62" s="67"/>
@@ -6111,7 +6111,7 @@
         <v>329.99317020000001</v>
       </c>
       <c r="L62" s="67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>1.1120204353310026</v>
       </c>
       <c r="M62" s="67"/>
@@ -6119,7 +6119,7 @@
         <v>1133.0455320000001</v>
       </c>
       <c r="O62" s="67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>14.156264566295201</v>
       </c>
       <c r="P62" s="67"/>

</xml_diff>